<commit_message>
FIXED ~ Shifting Conditional Formats ~ Removing Conditional Formats ~ Copying Conditional Formats ~ Reset _dataType for cell when Cell.Clear() ~ Some leaks of Range Shifted Subscriptions.
ADDED
+ RangeExtensions functions Crop and Relative
+ Conditional formats compress function
+ While saving, the conditional formats will be compressed
+ When cleaning a range, the conditional formatting will be removed
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/ConditionalFormatting/CFMultipleConditions.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/ConditionalFormatting/CFMultipleConditions.xlsx
@@ -430,7 +430,11 @@
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:sheetData/>
+  <x:sheetData>
+    <x:row r="1" spans="1:1">
+      <x:c r="A1" s="0" t="s"/>
+    </x:row>
+  </x:sheetData>
   <x:conditionalFormatting sqref="A1:A10">
     <x:cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <x:formula>3</x:formula>

</xml_diff>

<commit_message>
* Changes by igitur review comments. * Fixed some memory leaks. * Fixed some cpu performance issues.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/ConditionalFormatting/CFMultipleConditions.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/ConditionalFormatting/CFMultipleConditions.xlsx
@@ -430,11 +430,7 @@
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:sheetData>
-    <x:row r="1" spans="1:1">
-      <x:c r="A1" s="0" t="s"/>
-    </x:row>
-  </x:sheetData>
+  <x:sheetData/>
   <x:conditionalFormatting sqref="A1:A10">
     <x:cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <x:formula>3</x:formula>

</xml_diff>